<commit_message>
added two lines of data
</commit_message>
<xml_diff>
--- a/testexcel.xlsx
+++ b/testexcel.xlsx
@@ -14,9 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddd</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -366,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -389,6 +393,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>